<commit_message>
added sonar cube & sonar scanner
</commit_message>
<xml_diff>
--- a/ADSDataDirect.Web/Templates/TrackingStrat.xlsx
+++ b/ADSDataDirect.Web/Templates/TrackingStrat.xlsx
@@ -228,7 +228,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -262,6 +262,30 @@
     <xf numFmtId="3" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -277,19 +301,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -329,7 +341,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{52ED0265-6B15-4608-933D-C78AF6A4FE6A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{52ED0265-6B15-4608-933D-C78AF6A4FE6A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -379,7 +391,7 @@
         <xdr:cNvPr id="6" name="Rectangle: Rounded Corners 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -448,7 +460,7 @@
         <xdr:cNvPr id="11" name="Straight Connector 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000A000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -495,7 +507,7 @@
         <xdr:cNvPr id="31" name="Rectangle: Rounded Corners 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -582,7 +594,7 @@
         <xdr:cNvPr id="32" name="Straight Connector 31">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000A000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -629,7 +641,7 @@
         <xdr:cNvPr id="33" name="Rectangle: Rounded Corners 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -698,7 +710,7 @@
         <xdr:cNvPr id="34" name="Straight Connector 33">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000A000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -745,7 +757,7 @@
         <xdr:cNvPr id="35" name="Rectangle: Rounded Corners 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000014000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000014000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -816,7 +828,7 @@
         <xdr:cNvPr id="36" name="Straight Connector 35">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000A000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -863,7 +875,7 @@
         <xdr:cNvPr id="13" name="Rectangle: Rounded Corners 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7311213E-D13A-4A72-8B37-37313BC0C902}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{7311213E-D13A-4A72-8B37-37313BC0C902}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -935,7 +947,7 @@
         <xdr:cNvPr id="17" name="Rectangle: Rounded Corners 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7311213E-D13A-4A72-8B37-37313BC0C902}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{7311213E-D13A-4A72-8B37-37313BC0C902}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1007,7 +1019,7 @@
         <xdr:cNvPr id="14" name="Straight Connector 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000A000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1326,10 +1338,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J54"/>
+  <dimension ref="A1:J68"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:J1"/>
+      <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1344,16 +1356,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
       <c r="I1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1385,10 +1397,10 @@
       <c r="B4" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="19" t="s">
+      <c r="I4" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="J4" s="17">
+      <c r="J4" s="25">
         <f>G21</f>
         <v>1.1870000000000001</v>
       </c>
@@ -1400,8 +1412,8 @@
       <c r="B5" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="19"/>
-      <c r="J5" s="17"/>
+      <c r="I5" s="27"/>
+      <c r="J5" s="25"/>
     </row>
     <row r="6" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
@@ -1410,10 +1422,10 @@
       <c r="B6" t="s">
         <v>15</v>
       </c>
-      <c r="I6" s="16" t="s">
+      <c r="I6" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="J6" s="18">
+      <c r="J6" s="26">
         <f>J21</f>
         <v>13.720957114784419</v>
       </c>
@@ -1425,8 +1437,8 @@
       <c r="B7" t="s">
         <v>16</v>
       </c>
-      <c r="I7" s="16"/>
-      <c r="J7" s="18"/>
+      <c r="I7" s="24"/>
+      <c r="J7" s="26"/>
     </row>
     <row r="8" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
@@ -1456,351 +1468,341 @@
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B16" s="22">
+      <c r="B16" s="18">
         <f>J2</f>
         <v>100000</v>
       </c>
-      <c r="C16" s="22"/>
+      <c r="C16" s="18"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B17" s="22"/>
-      <c r="C17" s="22"/>
+      <c r="B17" s="18"/>
+      <c r="C17" s="18"/>
     </row>
     <row r="19" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="22">
+      <c r="B19" s="18">
         <v>8651</v>
       </c>
-      <c r="C19" s="22"/>
-      <c r="E19" s="13" t="s">
+      <c r="C19" s="18"/>
+      <c r="E19" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="G19" s="14">
+      <c r="G19" s="20">
         <v>5000</v>
       </c>
-      <c r="I19" s="13" t="s">
+      <c r="I19" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="J19" s="14">
+      <c r="J19" s="20">
         <v>5000</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="22"/>
-      <c r="C20" s="22"/>
-      <c r="E20" s="13"/>
-      <c r="G20" s="14"/>
-      <c r="I20" s="13"/>
-      <c r="J20" s="14"/>
+      <c r="B20" s="18"/>
+      <c r="C20" s="18"/>
+      <c r="E20" s="19"/>
+      <c r="G20" s="20"/>
+      <c r="I20" s="19"/>
+      <c r="J20" s="20"/>
     </row>
     <row r="21" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="24">
+      <c r="B21" s="22">
         <v>1187</v>
       </c>
-      <c r="C21" s="24"/>
-      <c r="E21" s="13" t="s">
+      <c r="C21" s="22"/>
+      <c r="E21" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="G21" s="15">
+      <c r="G21" s="23">
         <f>B21/B16*100</f>
         <v>1.1870000000000001</v>
       </c>
-      <c r="I21" s="13" t="s">
+      <c r="I21" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="J21" s="15">
+      <c r="J21" s="23">
         <f>B21/B19*100</f>
         <v>13.720957114784419</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="24"/>
-      <c r="C22" s="24"/>
-      <c r="E22" s="13"/>
-      <c r="G22" s="15"/>
-      <c r="I22" s="13"/>
-      <c r="J22" s="15"/>
+      <c r="B22" s="22"/>
+      <c r="C22" s="22"/>
+      <c r="E22" s="19"/>
+      <c r="G22" s="23"/>
+      <c r="I22" s="19"/>
+      <c r="J22" s="23"/>
     </row>
     <row r="23" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="24" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B24" s="21">
+      <c r="B24" s="17">
         <v>10</v>
       </c>
-      <c r="C24" s="21"/>
-      <c r="H24" s="23">
+      <c r="C24" s="17"/>
+      <c r="H24" s="21">
         <v>5</v>
       </c>
       <c r="I24" s="7"/>
     </row>
     <row r="25" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B25" s="21"/>
-      <c r="C25" s="21"/>
-      <c r="H25" s="23"/>
+      <c r="B25" s="17"/>
+      <c r="C25" s="17"/>
+      <c r="H25" s="21"/>
       <c r="I25" s="7"/>
     </row>
     <row r="26" spans="1:10" ht="10.8" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="27" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D27" s="13" t="s">
+      <c r="D27" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="E27" s="13"/>
-      <c r="G27" s="14"/>
-      <c r="I27" s="13" t="s">
+      <c r="E27" s="19"/>
+      <c r="G27" s="20"/>
+      <c r="I27" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="J27" s="14"/>
+      <c r="J27" s="20"/>
     </row>
     <row r="28" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="6"/>
       <c r="C28" s="6"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="G28" s="14"/>
-      <c r="I28" s="13"/>
-      <c r="J28" s="14"/>
-    </row>
-    <row r="29" spans="1:10" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="A29" s="8" t="s">
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
+      <c r="G28" s="20"/>
+      <c r="I28" s="19"/>
+      <c r="J28" s="20"/>
+    </row>
+    <row r="29" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
+      <c r="G29" s="14"/>
+      <c r="I29" s="13"/>
+      <c r="J29" s="14"/>
+    </row>
+    <row r="30" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
+      <c r="G30" s="14"/>
+      <c r="I30" s="13"/>
+      <c r="J30" s="14"/>
+    </row>
+    <row r="31" spans="1:10" ht="22.8" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A31" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B29" s="8"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8"/>
-      <c r="F29" s="8"/>
-      <c r="G29" s="8"/>
-      <c r="H29" s="8"/>
-      <c r="I29" s="8"/>
-      <c r="J29" s="8" t="s">
+      <c r="B31" s="8"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="8"/>
+      <c r="F31" s="8"/>
+      <c r="G31" s="8"/>
+      <c r="H31" s="8"/>
+      <c r="I31" s="8"/>
+      <c r="J31" s="8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="12" t="s">
+    <row r="32" spans="1:10" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="B30" s="12"/>
-      <c r="C30" s="12"/>
-      <c r="D30" s="12"/>
-      <c r="E30" s="12"/>
-      <c r="F30" s="12"/>
-      <c r="G30" s="12"/>
-      <c r="H30" s="12"/>
-      <c r="I30" s="12"/>
-      <c r="J30" s="10">
+      <c r="B32" s="28"/>
+      <c r="C32" s="28"/>
+      <c r="D32" s="28"/>
+      <c r="E32" s="28"/>
+      <c r="F32" s="28"/>
+      <c r="G32" s="28"/>
+      <c r="H32" s="28"/>
+      <c r="I32" s="28"/>
+      <c r="J32" s="10">
         <v>123</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="12"/>
-      <c r="B31" s="12"/>
-      <c r="C31" s="12"/>
-      <c r="D31" s="12"/>
-      <c r="E31" s="12"/>
-      <c r="F31" s="12"/>
-      <c r="G31" s="12"/>
-      <c r="H31" s="12"/>
-      <c r="I31" s="12"/>
-      <c r="J31" s="10" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="12"/>
-      <c r="B32" s="12"/>
-      <c r="C32" s="12"/>
-      <c r="D32" s="12"/>
-      <c r="E32" s="12"/>
-      <c r="F32" s="12"/>
-      <c r="G32" s="12"/>
-      <c r="H32" s="12"/>
-      <c r="I32" s="12"/>
-      <c r="J32" s="10" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="12"/>
-      <c r="B33" s="12"/>
-      <c r="C33" s="12"/>
-      <c r="D33" s="12"/>
-      <c r="E33" s="12"/>
-      <c r="F33" s="12"/>
-      <c r="G33" s="12"/>
-      <c r="H33" s="12"/>
-      <c r="I33" s="12"/>
+    <row r="33" spans="1:10" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="28"/>
+      <c r="B33" s="28"/>
+      <c r="C33" s="28"/>
+      <c r="D33" s="28"/>
+      <c r="E33" s="28"/>
+      <c r="F33" s="28"/>
+      <c r="G33" s="28"/>
+      <c r="H33" s="28"/>
+      <c r="I33" s="28"/>
       <c r="J33" s="10" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="12"/>
-      <c r="B34" s="12"/>
-      <c r="C34" s="12"/>
-      <c r="D34" s="12"/>
-      <c r="E34" s="12"/>
-      <c r="F34" s="12"/>
-      <c r="G34" s="12"/>
-      <c r="H34" s="12"/>
-      <c r="I34" s="12"/>
+    <row r="34" spans="1:10" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="28"/>
+      <c r="B34" s="28"/>
+      <c r="C34" s="28"/>
+      <c r="D34" s="28"/>
+      <c r="E34" s="28"/>
+      <c r="F34" s="28"/>
+      <c r="G34" s="28"/>
+      <c r="H34" s="28"/>
+      <c r="I34" s="28"/>
       <c r="J34" s="10" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="12"/>
-      <c r="B35" s="12"/>
-      <c r="C35" s="12"/>
-      <c r="D35" s="12"/>
-      <c r="E35" s="12"/>
-      <c r="F35" s="12"/>
-      <c r="G35" s="12"/>
-      <c r="H35" s="12"/>
-      <c r="I35" s="12"/>
+    <row r="35" spans="1:10" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="28"/>
+      <c r="B35" s="28"/>
+      <c r="C35" s="28"/>
+      <c r="D35" s="28"/>
+      <c r="E35" s="28"/>
+      <c r="F35" s="28"/>
+      <c r="G35" s="28"/>
+      <c r="H35" s="28"/>
+      <c r="I35" s="28"/>
       <c r="J35" s="10" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="12"/>
-      <c r="B36" s="12"/>
-      <c r="C36" s="12"/>
-      <c r="D36" s="12"/>
-      <c r="E36" s="12"/>
-      <c r="F36" s="12"/>
-      <c r="G36" s="12"/>
-      <c r="H36" s="12"/>
-      <c r="I36" s="12"/>
+    <row r="36" spans="1:10" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="28"/>
+      <c r="B36" s="28"/>
+      <c r="C36" s="28"/>
+      <c r="D36" s="28"/>
+      <c r="E36" s="28"/>
+      <c r="F36" s="28"/>
+      <c r="G36" s="28"/>
+      <c r="H36" s="28"/>
+      <c r="I36" s="28"/>
       <c r="J36" s="10" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="12"/>
-      <c r="B37" s="12"/>
-      <c r="C37" s="12"/>
-      <c r="D37" s="12"/>
-      <c r="E37" s="12"/>
-      <c r="F37" s="12"/>
-      <c r="G37" s="12"/>
-      <c r="H37" s="12"/>
-      <c r="I37" s="12"/>
+    <row r="37" spans="1:10" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="28"/>
+      <c r="B37" s="28"/>
+      <c r="C37" s="28"/>
+      <c r="D37" s="28"/>
+      <c r="E37" s="28"/>
+      <c r="F37" s="28"/>
+      <c r="G37" s="28"/>
+      <c r="H37" s="28"/>
+      <c r="I37" s="28"/>
       <c r="J37" s="10" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="12"/>
-      <c r="B38" s="12"/>
-      <c r="C38" s="12"/>
-      <c r="D38" s="12"/>
-      <c r="E38" s="12"/>
-      <c r="F38" s="12"/>
-      <c r="G38" s="12"/>
-      <c r="H38" s="12"/>
-      <c r="I38" s="12"/>
+    <row r="38" spans="1:10" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="28"/>
+      <c r="B38" s="28"/>
+      <c r="C38" s="28"/>
+      <c r="D38" s="28"/>
+      <c r="E38" s="28"/>
+      <c r="F38" s="28"/>
+      <c r="G38" s="28"/>
+      <c r="H38" s="28"/>
+      <c r="I38" s="28"/>
       <c r="J38" s="10" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="12"/>
-      <c r="B39" s="12"/>
-      <c r="C39" s="12"/>
-      <c r="D39" s="12"/>
-      <c r="E39" s="12"/>
-      <c r="F39" s="12"/>
-      <c r="G39" s="12"/>
-      <c r="H39" s="12"/>
-      <c r="I39" s="12"/>
+    <row r="39" spans="1:10" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="28"/>
+      <c r="B39" s="28"/>
+      <c r="C39" s="28"/>
+      <c r="D39" s="28"/>
+      <c r="E39" s="28"/>
+      <c r="F39" s="28"/>
+      <c r="G39" s="28"/>
+      <c r="H39" s="28"/>
+      <c r="I39" s="28"/>
       <c r="J39" s="10" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="12"/>
-      <c r="B40" s="12"/>
-      <c r="C40" s="12"/>
-      <c r="D40" s="12"/>
-      <c r="E40" s="12"/>
-      <c r="F40" s="12"/>
-      <c r="G40" s="12"/>
-      <c r="H40" s="12"/>
-      <c r="I40" s="12"/>
+    <row r="40" spans="1:10" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="28"/>
+      <c r="B40" s="28"/>
+      <c r="C40" s="28"/>
+      <c r="D40" s="28"/>
+      <c r="E40" s="28"/>
+      <c r="F40" s="28"/>
+      <c r="G40" s="28"/>
+      <c r="H40" s="28"/>
+      <c r="I40" s="28"/>
       <c r="J40" s="10" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="12"/>
-      <c r="B41" s="12"/>
-      <c r="C41" s="12"/>
-      <c r="D41" s="12"/>
-      <c r="E41" s="12"/>
-      <c r="F41" s="12"/>
-      <c r="G41" s="12"/>
-      <c r="H41" s="12"/>
-      <c r="I41" s="12"/>
+    <row r="41" spans="1:10" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="28"/>
+      <c r="B41" s="28"/>
+      <c r="C41" s="28"/>
+      <c r="D41" s="28"/>
+      <c r="E41" s="28"/>
+      <c r="F41" s="28"/>
+      <c r="G41" s="28"/>
+      <c r="H41" s="28"/>
+      <c r="I41" s="28"/>
       <c r="J41" s="10" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="12"/>
-      <c r="B42" s="12"/>
-      <c r="C42" s="12"/>
-      <c r="D42" s="12"/>
-      <c r="E42" s="12"/>
-      <c r="F42" s="12"/>
-      <c r="G42" s="12"/>
-      <c r="H42" s="12"/>
-      <c r="I42" s="12"/>
+    <row r="42" spans="1:10" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="28"/>
+      <c r="B42" s="28"/>
+      <c r="C42" s="28"/>
+      <c r="D42" s="28"/>
+      <c r="E42" s="28"/>
+      <c r="F42" s="28"/>
+      <c r="G42" s="28"/>
+      <c r="H42" s="28"/>
+      <c r="I42" s="28"/>
       <c r="J42" s="10" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="12"/>
-      <c r="B43" s="12"/>
-      <c r="C43" s="12"/>
-      <c r="D43" s="12"/>
-      <c r="E43" s="12"/>
-      <c r="F43" s="12"/>
-      <c r="G43" s="12"/>
-      <c r="H43" s="12"/>
-      <c r="I43" s="12"/>
+    <row r="43" spans="1:10" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="28"/>
+      <c r="B43" s="28"/>
+      <c r="C43" s="28"/>
+      <c r="D43" s="28"/>
+      <c r="E43" s="28"/>
+      <c r="F43" s="28"/>
+      <c r="G43" s="28"/>
+      <c r="H43" s="28"/>
+      <c r="I43" s="28"/>
       <c r="J43" s="10" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="12"/>
-      <c r="B44" s="12"/>
-      <c r="C44" s="12"/>
-      <c r="D44" s="12"/>
-      <c r="E44" s="12"/>
-      <c r="F44" s="12"/>
-      <c r="G44" s="12"/>
-      <c r="H44" s="12"/>
-      <c r="I44" s="12"/>
+    <row r="44" spans="1:10" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="28"/>
+      <c r="B44" s="28"/>
+      <c r="C44" s="28"/>
+      <c r="D44" s="28"/>
+      <c r="E44" s="28"/>
+      <c r="F44" s="28"/>
+      <c r="G44" s="28"/>
+      <c r="H44" s="28"/>
+      <c r="I44" s="28"/>
       <c r="J44" s="10" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="12"/>
-      <c r="B45" s="12"/>
-      <c r="C45" s="12"/>
-      <c r="D45" s="12"/>
-      <c r="E45" s="12"/>
-      <c r="F45" s="12"/>
-      <c r="G45" s="12"/>
-      <c r="H45" s="12"/>
-      <c r="I45" s="12"/>
+    <row r="45" spans="1:10" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="28"/>
+      <c r="B45" s="28"/>
+      <c r="C45" s="28"/>
+      <c r="D45" s="28"/>
+      <c r="E45" s="28"/>
+      <c r="F45" s="28"/>
+      <c r="G45" s="28"/>
+      <c r="H45" s="28"/>
+      <c r="I45" s="28"/>
       <c r="J45" s="10" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:10" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="12"/>
       <c r="B46" s="12"/>
       <c r="C46" s="12"/>
@@ -1810,11 +1812,9 @@
       <c r="G46" s="12"/>
       <c r="H46" s="12"/>
       <c r="I46" s="12"/>
-      <c r="J46" s="10" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J46" s="10"/>
+    </row>
+    <row r="47" spans="1:10" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="12"/>
       <c r="B47" s="12"/>
       <c r="C47" s="12"/>
@@ -1824,11 +1824,9 @@
       <c r="G47" s="12"/>
       <c r="H47" s="12"/>
       <c r="I47" s="12"/>
-      <c r="J47" s="10" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J47" s="10"/>
+    </row>
+    <row r="48" spans="1:10" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="12"/>
       <c r="B48" s="12"/>
       <c r="C48" s="12"/>
@@ -1838,11 +1836,9 @@
       <c r="G48" s="12"/>
       <c r="H48" s="12"/>
       <c r="I48" s="12"/>
-      <c r="J48" s="10" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J48" s="10"/>
+    </row>
+    <row r="49" spans="1:10" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="12"/>
       <c r="B49" s="12"/>
       <c r="C49" s="12"/>
@@ -1852,11 +1848,9 @@
       <c r="G49" s="12"/>
       <c r="H49" s="12"/>
       <c r="I49" s="12"/>
-      <c r="J49" s="10" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J49" s="10"/>
+    </row>
+    <row r="50" spans="1:10" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="12"/>
       <c r="B50" s="12"/>
       <c r="C50" s="12"/>
@@ -1866,11 +1860,9 @@
       <c r="G50" s="12"/>
       <c r="H50" s="12"/>
       <c r="I50" s="12"/>
-      <c r="J50" s="10" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J50" s="10"/>
+    </row>
+    <row r="51" spans="1:10" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="12"/>
       <c r="B51" s="12"/>
       <c r="C51" s="12"/>
@@ -1880,11 +1872,9 @@
       <c r="G51" s="12"/>
       <c r="H51" s="12"/>
       <c r="I51" s="12"/>
-      <c r="J51" s="10" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J51" s="10"/>
+    </row>
+    <row r="52" spans="1:10" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="12"/>
       <c r="B52" s="12"/>
       <c r="C52" s="12"/>
@@ -1894,11 +1884,9 @@
       <c r="G52" s="12"/>
       <c r="H52" s="12"/>
       <c r="I52" s="12"/>
-      <c r="J52" s="10" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J52" s="10"/>
+    </row>
+    <row r="53" spans="1:10" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="12"/>
       <c r="B53" s="12"/>
       <c r="C53" s="12"/>
@@ -1908,26 +1896,248 @@
       <c r="G53" s="12"/>
       <c r="H53" s="12"/>
       <c r="I53" s="12"/>
-      <c r="J53" s="10" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="A54" s="8" t="s">
+      <c r="J53" s="10"/>
+    </row>
+    <row r="54" spans="1:10" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="12"/>
+      <c r="B54" s="12"/>
+      <c r="C54" s="12"/>
+      <c r="D54" s="12"/>
+      <c r="E54" s="12"/>
+      <c r="F54" s="12"/>
+      <c r="G54" s="12"/>
+      <c r="H54" s="12"/>
+      <c r="I54" s="12"/>
+      <c r="J54" s="10"/>
+    </row>
+    <row r="55" spans="1:10" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="12"/>
+      <c r="B55" s="12"/>
+      <c r="C55" s="12"/>
+      <c r="D55" s="12"/>
+      <c r="E55" s="12"/>
+      <c r="F55" s="12"/>
+      <c r="G55" s="12"/>
+      <c r="H55" s="12"/>
+      <c r="I55" s="12"/>
+      <c r="J55" s="10"/>
+    </row>
+    <row r="56" spans="1:10" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="28"/>
+      <c r="B56" s="28"/>
+      <c r="C56" s="28"/>
+      <c r="D56" s="28"/>
+      <c r="E56" s="28"/>
+      <c r="F56" s="28"/>
+      <c r="G56" s="28"/>
+      <c r="H56" s="28"/>
+      <c r="I56" s="28"/>
+      <c r="J56" s="10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="28"/>
+      <c r="B57" s="28"/>
+      <c r="C57" s="28"/>
+      <c r="D57" s="28"/>
+      <c r="E57" s="28"/>
+      <c r="F57" s="28"/>
+      <c r="G57" s="28"/>
+      <c r="H57" s="28"/>
+      <c r="I57" s="28"/>
+      <c r="J57" s="10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="28"/>
+      <c r="B58" s="28"/>
+      <c r="C58" s="28"/>
+      <c r="D58" s="28"/>
+      <c r="E58" s="28"/>
+      <c r="F58" s="28"/>
+      <c r="G58" s="28"/>
+      <c r="H58" s="28"/>
+      <c r="I58" s="28"/>
+      <c r="J58" s="10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="28"/>
+      <c r="B59" s="28"/>
+      <c r="C59" s="28"/>
+      <c r="D59" s="28"/>
+      <c r="E59" s="28"/>
+      <c r="F59" s="28"/>
+      <c r="G59" s="28"/>
+      <c r="H59" s="28"/>
+      <c r="I59" s="28"/>
+      <c r="J59" s="10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="28"/>
+      <c r="B60" s="28"/>
+      <c r="C60" s="28"/>
+      <c r="D60" s="28"/>
+      <c r="E60" s="28"/>
+      <c r="F60" s="28"/>
+      <c r="G60" s="28"/>
+      <c r="H60" s="28"/>
+      <c r="I60" s="28"/>
+      <c r="J60" s="10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="28"/>
+      <c r="B61" s="28"/>
+      <c r="C61" s="28"/>
+      <c r="D61" s="28"/>
+      <c r="E61" s="28"/>
+      <c r="F61" s="28"/>
+      <c r="G61" s="28"/>
+      <c r="H61" s="28"/>
+      <c r="I61" s="28"/>
+      <c r="J61" s="10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="28"/>
+      <c r="B62" s="28"/>
+      <c r="C62" s="28"/>
+      <c r="D62" s="28"/>
+      <c r="E62" s="28"/>
+      <c r="F62" s="28"/>
+      <c r="G62" s="28"/>
+      <c r="H62" s="28"/>
+      <c r="I62" s="28"/>
+      <c r="J62" s="10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="28"/>
+      <c r="B63" s="28"/>
+      <c r="C63" s="28"/>
+      <c r="D63" s="28"/>
+      <c r="E63" s="28"/>
+      <c r="F63" s="28"/>
+      <c r="G63" s="28"/>
+      <c r="H63" s="28"/>
+      <c r="I63" s="28"/>
+      <c r="J63" s="10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="15"/>
+      <c r="B64" s="15"/>
+      <c r="C64" s="15"/>
+      <c r="D64" s="15"/>
+      <c r="E64" s="15"/>
+      <c r="F64" s="15"/>
+      <c r="G64" s="15"/>
+      <c r="H64" s="15"/>
+      <c r="I64" s="15"/>
+      <c r="J64" s="10"/>
+    </row>
+    <row r="65" spans="1:10" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="28"/>
+      <c r="B65" s="28"/>
+      <c r="C65" s="28"/>
+      <c r="D65" s="28"/>
+      <c r="E65" s="28"/>
+      <c r="F65" s="28"/>
+      <c r="G65" s="28"/>
+      <c r="H65" s="28"/>
+      <c r="I65" s="28"/>
+      <c r="J65" s="10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="15"/>
+      <c r="B66" s="15"/>
+      <c r="C66" s="15"/>
+      <c r="D66" s="15"/>
+      <c r="E66" s="15"/>
+      <c r="F66" s="15"/>
+      <c r="G66" s="15"/>
+      <c r="H66" s="15"/>
+      <c r="I66" s="15"/>
+      <c r="J66" s="10"/>
+    </row>
+    <row r="67" spans="1:10" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="28"/>
+      <c r="B67" s="28"/>
+      <c r="C67" s="28"/>
+      <c r="D67" s="28"/>
+      <c r="E67" s="28"/>
+      <c r="F67" s="28"/>
+      <c r="G67" s="28"/>
+      <c r="H67" s="28"/>
+      <c r="I67" s="28"/>
+      <c r="J67" s="10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" ht="25.8" x14ac:dyDescent="0.5">
+      <c r="A68" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B54" s="8"/>
-      <c r="C54" s="8"/>
-      <c r="D54" s="8"/>
-      <c r="E54" s="8"/>
-      <c r="F54" s="8"/>
-      <c r="G54" s="8"/>
-      <c r="H54" s="8"/>
-      <c r="I54" s="8"/>
-      <c r="J54" s="8"/>
+      <c r="B68" s="8"/>
+      <c r="C68" s="8"/>
+      <c r="D68" s="8"/>
+      <c r="E68" s="8"/>
+      <c r="F68" s="8"/>
+      <c r="G68" s="8"/>
+      <c r="H68" s="8"/>
+      <c r="I68" s="8"/>
+      <c r="J68" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="46">
+    <mergeCell ref="A62:I62"/>
+    <mergeCell ref="A63:I63"/>
+    <mergeCell ref="A65:I65"/>
+    <mergeCell ref="A67:I67"/>
+    <mergeCell ref="A57:I57"/>
+    <mergeCell ref="A58:I58"/>
+    <mergeCell ref="A59:I59"/>
+    <mergeCell ref="A60:I60"/>
+    <mergeCell ref="A61:I61"/>
+    <mergeCell ref="A42:I42"/>
+    <mergeCell ref="A43:I43"/>
+    <mergeCell ref="A44:I44"/>
+    <mergeCell ref="A45:I45"/>
+    <mergeCell ref="A56:I56"/>
+    <mergeCell ref="A37:I37"/>
+    <mergeCell ref="A38:I38"/>
+    <mergeCell ref="A39:I39"/>
+    <mergeCell ref="A40:I40"/>
+    <mergeCell ref="A41:I41"/>
+    <mergeCell ref="A32:I32"/>
+    <mergeCell ref="A33:I33"/>
+    <mergeCell ref="A34:I34"/>
+    <mergeCell ref="A35:I35"/>
+    <mergeCell ref="A36:I36"/>
+    <mergeCell ref="D27:E28"/>
+    <mergeCell ref="I19:I20"/>
+    <mergeCell ref="J19:J20"/>
+    <mergeCell ref="I21:I22"/>
+    <mergeCell ref="J21:J22"/>
+    <mergeCell ref="I6:I7"/>
+    <mergeCell ref="J4:J5"/>
+    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="I4:I5"/>
+    <mergeCell ref="G27:G28"/>
+    <mergeCell ref="I27:I28"/>
+    <mergeCell ref="J27:J28"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="B24:C25"/>
     <mergeCell ref="B19:C20"/>
@@ -1938,44 +2148,8 @@
     <mergeCell ref="E21:E22"/>
     <mergeCell ref="G21:G22"/>
     <mergeCell ref="B16:C17"/>
-    <mergeCell ref="I6:I7"/>
-    <mergeCell ref="J4:J5"/>
-    <mergeCell ref="J6:J7"/>
-    <mergeCell ref="I4:I5"/>
-    <mergeCell ref="G27:G28"/>
-    <mergeCell ref="I27:I28"/>
-    <mergeCell ref="J27:J28"/>
-    <mergeCell ref="D27:E28"/>
-    <mergeCell ref="I19:I20"/>
-    <mergeCell ref="J19:J20"/>
-    <mergeCell ref="I21:I22"/>
-    <mergeCell ref="J21:J22"/>
-    <mergeCell ref="A30:I30"/>
-    <mergeCell ref="A31:I31"/>
-    <mergeCell ref="A32:I32"/>
-    <mergeCell ref="A33:I33"/>
-    <mergeCell ref="A34:I34"/>
-    <mergeCell ref="A35:I35"/>
-    <mergeCell ref="A36:I36"/>
-    <mergeCell ref="A37:I37"/>
-    <mergeCell ref="A38:I38"/>
-    <mergeCell ref="A39:I39"/>
-    <mergeCell ref="A40:I40"/>
-    <mergeCell ref="A41:I41"/>
-    <mergeCell ref="A42:I42"/>
-    <mergeCell ref="A43:I43"/>
-    <mergeCell ref="A44:I44"/>
-    <mergeCell ref="A50:I50"/>
-    <mergeCell ref="A51:I51"/>
-    <mergeCell ref="A52:I52"/>
-    <mergeCell ref="A53:I53"/>
-    <mergeCell ref="A45:I45"/>
-    <mergeCell ref="A46:I46"/>
-    <mergeCell ref="A47:I47"/>
-    <mergeCell ref="A48:I48"/>
-    <mergeCell ref="A49:I49"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.3" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>

</xml_diff>